<commit_message>
Map interface - HashTable
</commit_message>
<xml_diff>
--- a/13 July 18/Classes and Interfaces inutil package.xlsx
+++ b/13 July 18/Classes and Interfaces inutil package.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="7755" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="7755" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="interfaces" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="144">
   <si>
     <t xml:space="preserve">Collection </t>
   </si>
@@ -320,9 +320,6 @@
     <t>SortedMap     [i]</t>
   </si>
   <si>
-    <t>NavigableMap</t>
-  </si>
-  <si>
     <t>The Collection hierarchy</t>
   </si>
   <si>
@@ -483,6 +480,9 @@
   </si>
   <si>
     <t>Not Allowed</t>
+  </si>
+  <si>
+    <t>NavigableMap [i]</t>
   </si>
 </sst>
 </file>
@@ -2005,14 +2005,14 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>57151</xdr:rowOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>857250</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2021,7 +2021,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="3714750" y="2238376"/>
+          <a:off x="1676400" y="5448301"/>
           <a:ext cx="733425" cy="19049"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2049,14 +2049,14 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>161926</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>847725</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2065,7 +2065,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3752851" y="2447925"/>
+          <a:off x="1714501" y="5667375"/>
           <a:ext cx="685799" cy="19050"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -2175,6 +2175,53 @@
         </a:fillRef>
         <a:effectRef idx="0">
           <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="31" name="Straight Arrow Connector 30"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2971800" y="4762501"/>
+          <a:ext cx="9525" cy="180974"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent5"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="tx1"/>
@@ -2765,8 +2812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2777,7 +2824,7 @@
     <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
   </cols>
@@ -2785,7 +2832,7 @@
     <row r="1" spans="1:12" ht="15.75" thickBot="1"/>
     <row r="2" spans="1:12" ht="15.75" thickBot="1">
       <c r="F2" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" thickBot="1">
@@ -3026,7 +3073,7 @@
       <c r="G17" s="20"/>
       <c r="H17" s="20"/>
       <c r="I17" s="34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J17" s="35"/>
       <c r="K17" s="35"/>
@@ -3121,13 +3168,13 @@
       <c r="G24" s="18"/>
       <c r="H24" s="18"/>
       <c r="I24" s="12" t="s">
-        <v>89</v>
+        <v>143</v>
       </c>
       <c r="J24" s="18"/>
       <c r="K24" s="18"/>
       <c r="L24" s="7"/>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" ht="15.75" thickBot="1">
       <c r="A25" s="17"/>
       <c r="B25" s="18"/>
       <c r="C25" s="18"/>
@@ -3145,8 +3192,8 @@
       <c r="A26" s="17"/>
       <c r="B26" s="18"/>
       <c r="C26" s="18"/>
-      <c r="D26" s="18" t="s">
-        <v>83</v>
+      <c r="D26" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="E26" s="18"/>
       <c r="F26" s="18"/>
@@ -3161,12 +3208,9 @@
       <c r="A27" s="17"/>
       <c r="B27" s="18"/>
       <c r="C27" s="18"/>
-      <c r="D27" s="18" t="s">
-        <v>84</v>
-      </c>
       <c r="E27" s="18"/>
       <c r="F27" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G27" s="18"/>
       <c r="H27" s="18"/>
@@ -3181,7 +3225,9 @@
       <c r="A28" s="17"/>
       <c r="B28" s="18"/>
       <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
+      <c r="D28" s="18" t="s">
+        <v>83</v>
+      </c>
       <c r="E28" s="18"/>
       <c r="F28" s="18"/>
       <c r="G28" s="18"/>
@@ -3195,13 +3241,15 @@
       <c r="A29" s="19"/>
       <c r="B29" s="20"/>
       <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
+      <c r="D29" s="20" t="s">
+        <v>84</v>
+      </c>
       <c r="E29" s="20"/>
       <c r="F29" s="20"/>
       <c r="G29" s="20"/>
       <c r="H29" s="20"/>
       <c r="I29" s="34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J29" s="35"/>
       <c r="K29" s="35"/>
@@ -3234,122 +3282,122 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="27" t="s">
         <v>127</v>
-      </c>
-      <c r="B1" s="27" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="18" customHeight="1" thickBot="1">
       <c r="A2" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>93</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="18" customHeight="1" thickBot="1">
       <c r="A3" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="22" t="s">
         <v>95</v>
-      </c>
-      <c r="B3" s="22" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" customHeight="1" thickBot="1">
       <c r="A4" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="22" t="s">
         <v>97</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18" customHeight="1" thickBot="1">
       <c r="A5" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" s="22" t="s">
         <v>99</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" customHeight="1" thickBot="1">
       <c r="A6" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="22" t="s">
         <v>101</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18" customHeight="1" thickBot="1">
       <c r="A7" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" s="22" t="s">
         <v>103</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18" customHeight="1" thickBot="1">
       <c r="A8" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" s="22" t="s">
         <v>105</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18" customHeight="1" thickBot="1">
       <c r="A9" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" s="22" t="s">
         <v>107</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18" customHeight="1" thickBot="1">
       <c r="A10" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" s="22" t="s">
         <v>109</v>
-      </c>
-      <c r="B10" s="22" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18" customHeight="1" thickBot="1">
       <c r="A11" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="B11" s="22" t="s">
         <v>111</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18" customHeight="1" thickBot="1">
       <c r="A12" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" s="22" t="s">
         <v>113</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18" customHeight="1" thickBot="1">
       <c r="A13" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="B13" s="22" t="s">
         <v>115</v>
-      </c>
-      <c r="B13" s="22" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="18" customHeight="1" thickBot="1">
       <c r="A14" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="B14" s="22" t="s">
         <v>117</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="18" customHeight="1" thickBot="1">
       <c r="A15" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15" s="22" t="s">
         <v>119</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -3373,34 +3421,34 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" customHeight="1" thickBot="1">
       <c r="A1" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="27" t="s">
         <v>127</v>
-      </c>
-      <c r="B1" s="27" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" customHeight="1" thickBot="1">
       <c r="A2" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" s="25" t="s">
         <v>121</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" thickBot="1">
       <c r="A3" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" s="22" t="s">
         <v>123</v>
-      </c>
-      <c r="B3" s="22" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" customHeight="1" thickBot="1">
       <c r="A4" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" s="22" t="s">
         <v>125</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -3412,7 +3460,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -3425,7 +3473,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="21.75" thickBot="1">
       <c r="A1" s="37" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
@@ -3433,7 +3481,7 @@
     </row>
     <row r="3" spans="1:4" ht="15.75">
       <c r="A3" s="28" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B3" s="28" t="s">
         <v>77</v>
@@ -3447,72 +3495,72 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="29" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="B5" s="30" t="s">
-        <v>134</v>
-      </c>
       <c r="C5" s="30" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="B6" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="C6" s="30" t="s">
-        <v>136</v>
-      </c>
       <c r="D6" s="30" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="B7" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="C7" s="30" t="s">
         <v>138</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="D7" s="30" t="s">
         <v>139</v>
-      </c>
-      <c r="D7" s="30" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="B8" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="C8" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="D8" s="30" t="s">
         <v>142</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>142</v>
-      </c>
-      <c r="D8" s="30" t="s">
-        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>